<commit_message>
Im Jupyter Skript für 256 beta hinzugefügt
</commit_message>
<xml_diff>
--- a/Praktikum/PAP 2.2/256 - Röntgenfluoreszenz/Diagramme/Vergleichstabelle.xlsx
+++ b/Praktikum/PAP 2.2/256 - Röntgenfluoreszenz/Diagramme/Vergleichstabelle.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Stoff</t>
   </si>
@@ -90,13 +90,37 @@
     </r>
   </si>
   <si>
-    <t>Abw.</t>
-  </si>
-  <si>
     <t>Δ</t>
   </si>
   <si>
     <t>Kalibrierung</t>
+  </si>
+  <si>
+    <r>
+      <t>Abw. [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>Abw. [σ]</t>
   </si>
 </sst>
 </file>
@@ -138,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -151,17 +175,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -327,35 +340,100 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -673,81 +751,83 @@
   <dimension ref="B1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="3" max="6" width="7.140625" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="15" t="s">
+      <c r="E3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="16" t="s">
-        <v>14</v>
+      <c r="K3" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="27">
         <v>22</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="24">
         <v>4.43</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="16">
         <v>0.17</v>
       </c>
       <c r="F4" s="2">
         <v>4.5110000000000001</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="19">
         <f>((D4-F4)^2)^(1/2)/(E4)</f>
         <v>0.47647058823529648</v>
       </c>
@@ -760,243 +840,243 @@
       <c r="J4" s="2">
         <v>4.9320000000000004</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="19">
         <f>((H4-J4)^2)^(1/2)/(I4)</f>
         <v>0.90526315789473999</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="28">
         <v>26</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="25">
         <v>6.41</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="17">
         <v>0.15</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>6.4039999999999999</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="G5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="3">
         <v>7.05</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>0.18</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>7.0579999999999998</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="20">
         <f t="shared" ref="K5:K11" si="0">((H5-J5)^2)^(1/2)/(I5)</f>
         <v>4.4444444444444488E-2</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="28">
         <v>28</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="25">
         <v>7.5</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="17">
         <v>0.16</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>7.4779999999999998</v>
       </c>
-      <c r="G6" s="6">
-        <f t="shared" ref="G5:G11" si="1">((D6-F6)^2)^(1/2)/(E6)</f>
+      <c r="G6" s="20">
+        <f t="shared" ref="G6:G11" si="1">((D6-F6)^2)^(1/2)/(E6)</f>
         <v>0.13750000000000151</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>8.2899999999999991</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>0.17</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <v>8.625</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="20">
         <f t="shared" si="0"/>
         <v>1.9705882352941224</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="28">
         <v>29</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="25">
         <v>8.06</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="17">
         <v>0.16</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>8.048</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="20">
         <f t="shared" si="1"/>
         <v>7.5000000000002842E-2</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>8.93</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>0.17</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <v>8.9049999999999994</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="20">
         <f t="shared" si="0"/>
         <v>0.14705882352941385</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="28">
         <v>30</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="25">
         <v>8.68</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="17">
         <v>0.16</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>8.6389999999999993</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="20">
         <f t="shared" si="1"/>
         <v>0.25625000000000231</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>9.6300000000000008</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>0.16</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <v>9.5719999999999992</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="20">
         <f t="shared" si="0"/>
         <v>0.36250000000001004</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="28">
         <v>40</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="25">
         <v>15.81</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="17">
         <v>0.16</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>15.78</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="20">
         <f t="shared" si="1"/>
         <v>0.18750000000000711</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>17.96</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>0.18</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="4">
         <v>17.670000000000002</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="20">
         <f t="shared" si="0"/>
         <v>1.6111111111111065</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="28">
         <v>42</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="25">
         <v>17.48</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="17">
         <v>0.17</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>17.48</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="4">
+      <c r="G10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="3">
         <v>19.59</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>0.21</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="4">
         <v>19.61</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="20">
         <f t="shared" si="0"/>
         <v>9.5238095238093207E-2</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="29">
         <v>47</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="26">
         <v>21.96</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="18">
         <v>0.17</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <v>22.16</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="21">
         <f t="shared" si="1"/>
         <v>1.1764705882352899</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>24.56</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="7">
         <v>0.13</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="7">
         <v>24.94</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="21">
         <f t="shared" si="0"/>
         <v>2.9230769230769424</v>
       </c>
@@ -1007,6 +1087,6 @@
     <mergeCell ref="H2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>